<commit_message>
HotFix: Class: -Private class variables -Init -Getter
Comments

Product BackLog
</commit_message>
<xml_diff>
--- a/Product Backlog/Product BackLog.xlsx
+++ b/Product Backlog/Product BackLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarevok\IdeaProjects\SEM-Project\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61891070-3CDD-4604-928F-80626B1BA79B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E0C789-EE47-437D-A762-03331A073F61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E44FCAF2-05EF-4A3E-9388-0D83F859B995}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Create and connect to world database</t>
+  </si>
+  <si>
+    <t>2hr</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Show the list</t>
+  </si>
+  <si>
+    <t>Show the list with Limit</t>
   </si>
 </sst>
 </file>
@@ -670,15 +682,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,6 +690,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1020,7 +1032,7 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1048,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="27"/>
@@ -1048,10 +1060,10 @@
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
       <c r="J1" s="28"/>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="37"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1092,8 +1104,8 @@
       <c r="B3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="38" t="s">
-        <v>12</v>
+      <c r="C3" s="35" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>14</v>
@@ -1110,7 +1122,7 @@
       <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="36" t="s">
         <v>68</v>
       </c>
       <c r="J3" s="7" t="s">
@@ -1139,11 +1151,21 @@
       <c r="E4" s="11">
         <v>100</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="7"/>
+      <c r="F4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -1167,11 +1189,21 @@
       <c r="E5" s="11">
         <v>100</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="7"/>
+      <c r="F5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -1189,11 +1221,21 @@
       <c r="E6" s="11">
         <v>100</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="7"/>
+      <c r="F6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="L6" s="14" t="s">
         <v>14</v>
       </c>
@@ -1217,11 +1259,21 @@
       <c r="E7" s="11">
         <v>100</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
+      <c r="F7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L7" s="15" t="s">
         <v>16</v>
       </c>
@@ -1245,11 +1297,21 @@
       <c r="E8" s="11">
         <v>100</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
+      <c r="F8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L8" s="16" t="s">
         <v>18</v>
       </c>
@@ -1273,11 +1335,21 @@
       <c r="E9" s="11">
         <v>100</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
+      <c r="F9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1295,11 +1367,21 @@
       <c r="E10" s="11">
         <v>100</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="7"/>
+      <c r="F10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -1317,11 +1399,21 @@
       <c r="E11" s="11">
         <v>100</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
+      <c r="F11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -1339,11 +1431,21 @@
       <c r="E12" s="11">
         <v>100</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="7"/>
+      <c r="F12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -1361,11 +1463,21 @@
       <c r="E13" s="11">
         <v>100</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="7"/>
+      <c r="F13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
@@ -1383,11 +1495,21 @@
       <c r="E14" s="11">
         <v>100</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
+      <c r="F14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1405,11 +1527,21 @@
       <c r="E15" s="11">
         <v>100</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
+      <c r="F15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -1427,11 +1559,21 @@
       <c r="E16" s="11">
         <v>100</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="7"/>
+      <c r="F16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -1449,11 +1591,21 @@
       <c r="E17" s="11">
         <v>100</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="7"/>
+      <c r="F17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -1471,11 +1623,21 @@
       <c r="E18" s="11">
         <v>100</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
+      <c r="F18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
@@ -1493,11 +1655,21 @@
       <c r="E19" s="11">
         <v>100</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="7"/>
+      <c r="F19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -2006,7 +2178,9 @@
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
       <c r="B43" s="24"/>
       <c r="C43" s="33"/>
       <c r="D43" s="34"/>
@@ -2018,7 +2192,9 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="6">
+        <v>42</v>
+      </c>
       <c r="B44" s="24"/>
       <c r="C44" s="33"/>
       <c r="D44" s="20"/>
@@ -2030,7 +2206,9 @@
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="6">
+        <v>43</v>
+      </c>
       <c r="B45" s="24"/>
       <c r="C45" s="33"/>
       <c r="D45" s="34"/>
@@ -2042,7 +2220,9 @@
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="6">
+        <v>44</v>
+      </c>
       <c r="B46" s="24"/>
       <c r="C46" s="33"/>
       <c r="D46" s="20"/>
@@ -2054,7 +2234,9 @@
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="6">
+        <v>45</v>
+      </c>
       <c r="B47" s="24"/>
       <c r="C47" s="33"/>
       <c r="D47" s="34"/>
@@ -2066,7 +2248,9 @@
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
       <c r="B48" s="24"/>
       <c r="C48" s="33"/>
       <c r="D48" s="20"/>
@@ -2078,7 +2262,9 @@
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="6">
+        <v>47</v>
+      </c>
       <c r="B49" s="24"/>
       <c r="C49" s="33"/>
       <c r="D49" s="34"/>
@@ -2090,7 +2276,9 @@
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="6">
+        <v>48</v>
+      </c>
       <c r="B50" s="24"/>
       <c r="C50" s="33"/>
       <c r="D50" s="20"/>
@@ -2102,7 +2290,9 @@
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
       <c r="B51" s="24"/>
       <c r="C51" s="33"/>
       <c r="D51" s="34"/>
@@ -2114,7 +2304,9 @@
       <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+      <c r="A52" s="6">
+        <v>50</v>
+      </c>
       <c r="B52" s="24"/>
       <c r="C52" s="33"/>
       <c r="D52" s="20"/>
@@ -2126,7 +2318,9 @@
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+      <c r="A53" s="6">
+        <v>51</v>
+      </c>
       <c r="B53" s="24"/>
       <c r="C53" s="33"/>
       <c r="D53" s="34"/>
@@ -2138,7 +2332,9 @@
       <c r="J53" s="7"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
+      <c r="A54" s="6">
+        <v>52</v>
+      </c>
       <c r="B54" s="24"/>
       <c r="C54" s="33"/>
       <c r="D54" s="20"/>
@@ -2150,7 +2346,9 @@
       <c r="J54" s="7"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
+      <c r="A55" s="6">
+        <v>53</v>
+      </c>
       <c r="B55" s="24"/>
       <c r="C55" s="33"/>
       <c r="D55" s="34"/>
@@ -2162,7 +2360,9 @@
       <c r="J55" s="7"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+      <c r="A56" s="6">
+        <v>54</v>
+      </c>
       <c r="B56" s="24"/>
       <c r="C56" s="33"/>
       <c r="D56" s="20"/>
@@ -2174,7 +2374,9 @@
       <c r="J56" s="7"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
+      <c r="A57" s="6">
+        <v>55</v>
+      </c>
       <c r="B57" s="24"/>
       <c r="C57" s="33"/>
       <c r="D57" s="34"/>
@@ -2186,7 +2388,9 @@
       <c r="J57" s="7"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="6">
+        <v>56</v>
+      </c>
       <c r="B58" s="24"/>
       <c r="C58" s="33"/>
       <c r="D58" s="20"/>
@@ -2255,11 +2459,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -2386,6 +2590,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE714F029A1944498C1187C71CE6A5C9" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dacc76c05fba1b052c3bd8a4917f913">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="664c1d2d-403e-4aaa-9b5b-d84cdff106bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71f88469e4631bff9119aa4fa50f9994" ns3:_="">
     <xsd:import namespace="664c1d2d-403e-4aaa-9b5b-d84cdff106bd"/>
@@ -2531,22 +2750,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB3C35AE-725D-4BBE-9212-E87DD20A09D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="664c1d2d-403e-4aaa-9b5b-d84cdff106bd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A39DAE-FACF-4DF3-A9E3-884FE7F8BD96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4352C1E-1FBC-41B0-9750-9E20D34F1EF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2562,28 +2790,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A39DAE-FACF-4DF3-A9E3-884FE7F8BD96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB3C35AE-725D-4BBE-9212-E87DD20A09D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="664c1d2d-403e-4aaa-9b5b-d84cdff106bd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>